<commit_message>
check if average is used for lung SBRT
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/sein.xlsx
+++ b/Plancheck/check_protocol/sein.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="2"/>
   </bookViews>
@@ -13,7 +13,7 @@
     <sheet name="couch_structures" sheetId="4" r:id="rId4"/>
     <sheet name="Doses" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -418,9 +418,6 @@
     <t>PTVsein-PTVboost</t>
   </si>
   <si>
-    <t>Ring_PTVboost</t>
-  </si>
-  <si>
     <t>Seuillage</t>
   </si>
   <si>
@@ -457,13 +454,16 @@
     <t>D2%&lt;107%</t>
   </si>
   <si>
-    <t>Ring_PTVsein</t>
+    <t>RingPTVsein</t>
+  </si>
+  <si>
+    <t>RingPTVboost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1143,11 +1143,11 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -2438,7 +2438,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2516,7 +2516,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -2527,7 +2527,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2691,31 +2691,31 @@
         <v>116</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2723,7 +2723,7 @@
         <v>124</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -2737,10 +2737,10 @@
         <v>94</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="E5" s="6"/>
     </row>

</xml_diff>